<commit_message>
salto doesn't work perfect
</commit_message>
<xml_diff>
--- a/choreography/routines/routine_act_salto.xlsx
+++ b/choreography/routines/routine_act_salto.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="285">
   <si>
     <t xml:space="preserve">Start time</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t xml:space="preserve">OFF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">true</t>
   </si>
   <si>
     <t xml:space="preserve">Iets spanning zodat benen niet overklappen</t>
@@ -1466,7 +1469,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="G6" activeCellId="0" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.75" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1598,7 +1601,7 @@
         <v>11</v>
       </c>
       <c r="G4" s="5" t="n">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="H4" s="5" t="n">
         <v>0</v>
@@ -1630,10 +1633,10 @@
         <v>33</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="G5" s="5" t="n">
-        <v>45</v>
+        <v>75</v>
       </c>
       <c r="H5" s="5" t="n">
         <v>0</v>
@@ -1642,7 +1645,7 @@
         <v>0.15</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1658,7 +1661,7 @@
         <v>9</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E6" s="8" t="str">
         <f aca="false">INDEX(movelist!B:B, MATCH($D6, movelist!A:A, 0))</f>
@@ -1668,7 +1671,7 @@
         <v>11</v>
       </c>
       <c r="G6" s="5" t="n">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="H6" s="5" t="n">
         <v>30</v>
@@ -1691,7 +1694,7 @@
         <v>12</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" s="8" t="str">
         <f aca="false">INDEX(movelist!B:B, MATCH($D7, movelist!A:A, 0))</f>
@@ -1759,7 +1762,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E9" s="8" t="str">
         <f aca="false">INDEX(movelist!B:B, MATCH($D9, movelist!A:A, 0))</f>
@@ -1792,7 +1795,7 @@
         <v>12</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E10" s="8" t="str">
         <f aca="false">INDEX(movelist!B:B, MATCH($D10, movelist!A:A, 0))</f>
@@ -2255,178 +2258,178 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="15" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="15" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="15" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="15" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="15" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="15" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="15" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="15" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="15" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="15" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="15" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="15" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
+        <v>52</v>
+      </c>
+      <c r="B19" s="15" t="s">
         <v>51</v>
-      </c>
-      <c r="B19" s="15" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="15" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="15" t="s">
         <v>54</v>
-      </c>
-      <c r="B21" s="15" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2434,551 +2437,551 @@
         <v>10</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B25" s="16" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="16" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B26" s="16" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B27" s="16" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B28" s="16" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="16" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B29" s="16" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="16" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B30" s="16" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="16" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B31" s="16" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="16" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B32" s="16" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B33" s="16" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="16" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B34" s="16" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="16" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B35" s="16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="16" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B36" s="16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="16" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B37" s="16" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="16" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="16" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="16" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="16" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="16" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="16" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="16" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="16" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="16" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="16" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="16" t="s">
+        <v>103</v>
+      </c>
+      <c r="B48" s="16" t="s">
         <v>102</v>
-      </c>
-      <c r="B48" s="16" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="16" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="16" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="16" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="16" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="16" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="16" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="16" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="16" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="16" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="16" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="16" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="16" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="16" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="16" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="16" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="16" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="16" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="16" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="16" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="16" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="16" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="16" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="16" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="16" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="16" t="s">
+        <v>151</v>
+      </c>
+      <c r="B74" s="16" t="s">
         <v>150</v>
-      </c>
-      <c r="B74" s="16" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="16" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="16" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="16" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="16" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="16" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="16" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="B80" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="16" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B82" s="16" t="s">
         <v>164</v>
-      </c>
-      <c r="B82" s="16" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="16" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B83" s="16" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="16" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="16" t="s">
+        <v>170</v>
+      </c>
+      <c r="B85" s="16" t="s">
         <v>169</v>
-      </c>
-      <c r="B85" s="16" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="16" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="16" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="16" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="B88" s="16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="16" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="B89" s="16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="16" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B90" s="16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="16" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="B91" s="16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="16" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B92" s="16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2986,543 +2989,543 @@
         <v>13</v>
       </c>
       <c r="B93" s="16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="16" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="B94" s="16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="16" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B95" s="16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="16" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="B96" s="16" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="16" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B97" s="16" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="16" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B98" s="16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="16" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B99" s="16" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="16" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B100" s="16" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="B101" s="16" t="s">
         <v>187</v>
-      </c>
-      <c r="B101" s="16" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A102" s="16" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B102" s="16" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A103" s="16" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="B103" s="16" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="16" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B104" s="16" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="16" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B105" s="16" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="16" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="B106" s="16" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="16" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B107" s="16" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="16" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B108" s="16" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="16" t="s">
+        <v>199</v>
+      </c>
+      <c r="B109" s="16" t="s">
         <v>198</v>
-      </c>
-      <c r="B109" s="16" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="16" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B110" s="16" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A111" s="16" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B111" s="16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A112" s="16" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B112" s="16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="16" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B113" s="16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="16" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="B114" s="16" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="16" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B115" s="16" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="16" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B116" s="16" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="16" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="B117" s="16" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A118" s="16" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B118" s="16" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A119" s="16" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B119" s="16" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A120" s="16" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B120" s="16" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="16" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B121" s="16" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="16" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B122" s="16" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="16" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B123" s="16" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="16" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B124" s="16" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="16" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B125" s="16" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A126" s="16" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B126" s="16" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A127" s="16" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B127" s="16" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A128" s="16" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B128" s="16" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A129" s="16" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="B129" s="16" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A130" s="16" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="B130" s="16" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A131" s="16" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B131" s="16" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A132" s="16" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B132" s="16" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A133" s="16" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B133" s="16" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A134" s="16" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B134" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A135" s="16" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B135" s="16" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A136" s="16" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="B136" s="16" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A137" s="16" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B137" s="16" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A138" s="16" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B138" s="16" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A139" s="16" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="B139" s="16" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A140" s="16" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B140" s="16" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A141" s="16" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B141" s="16" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A142" s="16" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="B142" s="16" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A143" s="15" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="B143" s="16" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A144" s="15" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="B144" s="16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A145" s="15" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B145" s="16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A146" s="15" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="B146" s="16" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A147" s="15" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="B147" s="16" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A148" s="15" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B148" s="16" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A149" s="15" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="B149" s="16" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A150" s="15" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B150" s="16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A151" s="15" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B151" s="16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A152" s="15" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="B152" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A153" s="15" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B153" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A154" s="15" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B154" s="16" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A155" s="15" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B155" s="16" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A156" s="15" t="s">
+        <v>276</v>
+      </c>
+      <c r="B156" s="16" t="s">
         <v>275</v>
-      </c>
-      <c r="B156" s="16" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="15" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="B157" s="16" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A158" s="15" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B158" s="16" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A159" s="15" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="B159" s="16" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A160" s="15" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B160" s="16" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>

</xml_diff>